<commit_message>
Pridane texty a fotky od lubice, upravene nazvy stranok, trosku potriedene pluginy a podobne veci
</commit_message>
<xml_diff>
--- a/some-info/technik-dochadzka.xlsx
+++ b/some-info/technik-dochadzka.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoram_000\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\technik\some-info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,6 +483,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>41995</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Pridane texty a fotky od lubice, upravene nazvy stranok, trosku potriedene pluginy a podobne veci"
This reverts commit 5c9b0c731f692c8282af60c819a324cd084beb26.
</commit_message>
<xml_diff>
--- a/some-info/technik-dochadzka.xlsx
+++ b/some-info/technik-dochadzka.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\technik\some-info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoram_000\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,14 +483,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>41995</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.875</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
odstraneny problem v upcoming event - error pri loggond_only indexe
</commit_message>
<xml_diff>
--- a/some-info/technik-dochadzka.xlsx
+++ b/some-info/technik-dochadzka.xlsx
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,12 +527,17 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E9" s="4">
+      <c r="B9" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E14" s="4">
         <f>SUM(E2:E8)</f>
         <v>31.5</v>
       </c>
-      <c r="F9">
-        <f>E9*4</f>
+      <c r="F14">
+        <f>E14*4</f>
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
users zmeny, zobrazenie a rozdelenie podla tanecmhudbamspev secondary role
</commit_message>
<xml_diff>
--- a/some-info/technik-dochadzka.xlsx
+++ b/some-info/technik-dochadzka.xlsx
@@ -373,7 +373,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,6 +530,9 @@
       <c r="B9" s="2">
         <v>0.83333333333333337</v>
       </c>
+      <c r="C9" s="2">
+        <v>0.95833333333333337</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E14" s="4">

</xml_diff>

<commit_message>
upraveny edit profil page a edit event page v dashboarde tak aby sa nezmenili po update - pomocou jquery oheckovane
</commit_message>
<xml_diff>
--- a/some-info/technik-dochadzka.xlsx
+++ b/some-info/technik-dochadzka.xlsx
@@ -373,7 +373,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +523,8 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E8">
-        <v>12</v>
+        <f>12+4+4</f>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -533,15 +534,23 @@
       <c r="C9" s="2">
         <v>0.95833333333333337</v>
       </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E14" s="4">
         <f>SUM(E2:E8)</f>
-        <v>31.5</v>
+        <v>39.5</v>
       </c>
       <c r="F14">
         <f>E14*4</f>
-        <v>126</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>